<commit_message>
Changed the lookup of the config file using os, sys modules. Corrected bug in monitor() function of keysight DAQ
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
+++ b/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96BFE3D-F9AE-43CB-9266-7859853F4132}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AFB479-CB69-423C-AEB2-53E13B53CC3E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
@@ -322,6 +322,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -363,10 +366,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,7 +688,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +734,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
@@ -738,13 +742,15 @@
       <c r="C2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="3">
+        <f>0.95*F2</f>
+        <v>19.170999999999999</v>
+      </c>
+      <c r="E2" s="3">
+        <f>1.05*F2</f>
+        <v>21.189</v>
+      </c>
+      <c r="F2" s="3">
         <v>20.18</v>
       </c>
       <c r="H2" t="s">
@@ -754,7 +760,7 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>1+A2</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>60</v>
@@ -762,13 +768,15 @@
       <c r="C3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D9" si="0">0.95*F3</f>
+        <v>19.170999999999999</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E9" si="1">1.05*F3</f>
+        <v>21.189</v>
+      </c>
+      <c r="F3" s="3">
         <v>20.18</v>
       </c>
       <c r="H3" t="s">
@@ -777,8 +785,8 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A33" si="0">1+A3</f>
-        <v>3</v>
+        <f t="shared" ref="A4:A19" si="2">1+A3</f>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>61</v>
@@ -786,13 +794,15 @@
       <c r="C4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D4">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>30.4</v>
-      </c>
-      <c r="F4">
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>28.689999999999998</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>31.71</v>
+      </c>
+      <c r="F4" s="3">
         <v>30.2</v>
       </c>
       <c r="H4" t="s">
@@ -801,8 +811,8 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>69</v>
@@ -810,13 +820,15 @@
       <c r="C5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D5">
-        <v>30</v>
-      </c>
-      <c r="E5">
-        <v>30.4</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>28.689999999999998</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>31.71</v>
+      </c>
+      <c r="F5" s="3">
         <v>30.2</v>
       </c>
       <c r="H5" t="s">
@@ -825,8 +837,8 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>71</v>
@@ -834,13 +846,15 @@
       <c r="C6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>19.170999999999999</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>21.189</v>
+      </c>
+      <c r="F6" s="3">
         <v>20.18</v>
       </c>
       <c r="H6" t="s">
@@ -849,8 +863,8 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>72</v>
@@ -858,13 +872,15 @@
       <c r="C7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>19.170999999999999</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>21.189</v>
+      </c>
+      <c r="F7" s="3">
         <v>20.18</v>
       </c>
       <c r="H7" t="s">
@@ -873,8 +889,8 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>74</v>
@@ -882,13 +898,15 @@
       <c r="C8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D8">
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <v>30.4</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>28.689999999999998</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>31.71</v>
+      </c>
+      <c r="F8" s="3">
         <v>30.2</v>
       </c>
       <c r="H8" t="s">
@@ -897,8 +915,8 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>73</v>
@@ -906,13 +924,15 @@
       <c r="C9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D9">
-        <v>30</v>
-      </c>
-      <c r="E9">
-        <v>30.4</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>28.689999999999998</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>31.71</v>
+      </c>
+      <c r="F9" s="3">
         <v>30.2</v>
       </c>
       <c r="H9" t="s">
@@ -921,8 +941,8 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -945,8 +965,8 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -969,8 +989,8 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -993,8 +1013,8 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
@@ -1017,8 +1037,8 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -1043,8 +1063,8 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -1053,11 +1073,11 @@
         <v>35</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D19" si="1">0.9*F15</f>
+        <f t="shared" ref="D15:D19" si="3">0.9*F15</f>
         <v>5.5350000000000001</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E15:E19" si="2">1.1*F15</f>
+        <f t="shared" ref="E15:E19" si="4">1.1*F15</f>
         <v>6.7650000000000006</v>
       </c>
       <c r="F15">
@@ -1069,8 +1089,8 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -1079,11 +1099,11 @@
         <v>36</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5350000000000001</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.7650000000000006</v>
       </c>
       <c r="F16">
@@ -1095,8 +1115,8 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1105,11 +1125,11 @@
         <v>37</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5350000000000001</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.7650000000000006</v>
       </c>
       <c r="F17">
@@ -1121,8 +1141,8 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -1131,11 +1151,11 @@
         <v>38</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5350000000000001</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.7650000000000006</v>
       </c>
       <c r="F18">
@@ -1147,8 +1167,8 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1157,11 +1177,11 @@
         <v>39</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5350000000000001</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.7650000000000006</v>
       </c>
       <c r="F19">
@@ -1174,7 +1194,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>1+A19</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>91</v>
@@ -1197,8 +1217,8 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" ref="A21:A33" si="3">1+A20</f>
-        <v>20</v>
+        <f t="shared" ref="A21:A33" si="5">1+A20</f>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>92</v>
@@ -1221,8 +1241,8 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="3"/>
-        <v>21</v>
+        <f t="shared" si="5"/>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -1245,8 +1265,8 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="3"/>
-        <v>22</v>
+        <f t="shared" si="5"/>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
@@ -1269,8 +1289,8 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="3"/>
-        <v>23</v>
+        <f t="shared" si="5"/>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>21</v>
@@ -1293,8 +1313,8 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="3"/>
-        <v>24</v>
+        <f t="shared" si="5"/>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -1317,8 +1337,8 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f t="shared" si="5"/>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
@@ -1341,8 +1361,8 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="3"/>
-        <v>26</v>
+        <f t="shared" si="5"/>
+        <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>56</v>
@@ -1353,8 +1373,8 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="3"/>
-        <v>27</v>
+        <f t="shared" si="5"/>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
@@ -1377,8 +1397,8 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="3"/>
-        <v>28</v>
+        <f t="shared" si="5"/>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
@@ -1401,8 +1421,8 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="3"/>
-        <v>29</v>
+        <f t="shared" si="5"/>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
@@ -1425,8 +1445,8 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="3"/>
-        <v>30</v>
+        <f t="shared" si="5"/>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
@@ -1449,8 +1469,8 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="3"/>
-        <v>31</v>
+        <f t="shared" si="5"/>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>50</v>
@@ -1473,8 +1493,8 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="3"/>
-        <v>32</v>
+        <f t="shared" si="5"/>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
added to keysight monitor() function so that it can be called from any state. Adjusted cap discharge algorithm after fixing the hardware. Made HVCAP charging test more robust. I should wait for the HVCAP voltage to level off and use the steady state charge level as the measured value.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
+++ b/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AFB479-CB69-423C-AEB2-53E13B53CC3E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A1FC52-6FCA-47FB-A5D7-ACBFE3B49A93}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="1" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="95">
   <si>
     <t>TEST #</t>
   </si>
@@ -687,7 +687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA788C9-474B-4068-A04A-775EAB4B4CD4}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1523,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CEAD3C-E293-403D-9957-624DD4ECBBD6}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,7 +1535,7 @@
     <col min="3" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -1552,13 +1552,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>89</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -1574,14 +1577,14 @@
       <c r="E2">
         <v>24</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1597,14 +1600,14 @@
       <c r="E3">
         <v>24</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -1620,14 +1623,14 @@
       <c r="E4">
         <v>24</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -1643,14 +1646,14 @@
       <c r="E5">
         <v>24</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -1666,14 +1669,14 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1689,14 +1692,14 @@
       <c r="E7">
         <v>2.5</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -1712,14 +1715,14 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>1</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -1735,14 +1738,14 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1758,14 +1761,14 @@
       <c r="E10">
         <v>315</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>4</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -1781,14 +1784,14 @@
       <c r="E11">
         <v>240</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>4</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -1804,14 +1807,14 @@
       <c r="E12">
         <v>650</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>6</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -1827,14 +1830,14 @@
       <c r="E13">
         <v>16</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1850,14 +1853,14 @@
       <c r="E14">
         <v>24</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -1870,10 +1873,10 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>3.57</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tried to parameterize the sweep function which would check the 24V thresholds. But, the architecture doesn't really lend itself to that. So for now, each threshold check will be some copy/pasted code.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
+++ b/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A1FC52-6FCA-47FB-A5D7-ACBFE3B49A93}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C69357C-8C0B-4F55-B34B-FAC858B0F0B1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="1" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
   <si>
     <t>TEST #</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>HvBuckBootstrap2</t>
+  </si>
+  <si>
+    <t>RL1</t>
+  </si>
+  <si>
+    <t>RL2</t>
   </si>
 </sst>
 </file>
@@ -685,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA788C9-474B-4068-A04A-775EAB4B4CD4}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,7 +706,7 @@
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -731,8 +737,14 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -757,7 +769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>1+A2</f>
         <v>1</v>
@@ -783,7 +795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A19" si="2">1+A3</f>
         <v>2</v>
@@ -809,7 +821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -835,7 +847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -861,7 +873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -887,7 +899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -913,7 +925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -939,7 +951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -963,7 +975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -987,7 +999,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1011,7 +1023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -1035,7 +1047,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -1061,7 +1073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -1087,7 +1099,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -1526,7 +1538,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,7 +1650,7 @@
         <v>204</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>23.5</v>
       </c>
       <c r="D5">
         <v>24.5</v>

</xml_diff>

<commit_message>
realized the bootstrap test cannot be tested without allowing the buck to start up. Committing to get a snapshot of the attempt made before this realization.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
+++ b/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C69357C-8C0B-4F55-B34B-FAC858B0F0B1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761AEDA7-9F7A-445F-88CE-9536020F8CF4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="1" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
   <si>
     <t>TEST #</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>RL2</t>
+  </si>
+  <si>
+    <t>HV CAP REGULATION</t>
   </si>
 </sst>
 </file>
@@ -691,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA788C9-474B-4068-A04A-775EAB4B4CD4}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +800,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A19" si="2">1+A3</f>
+        <f t="shared" ref="A4:A34" si="2">1+A3</f>
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -1029,22 +1032,20 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C13" s="1"/>
       <c r="D13">
-        <v>950</v>
+        <v>0.1</v>
       </c>
       <c r="E13">
-        <v>1050</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1053,24 +1054,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D14">
-        <f>0.9*F14</f>
-        <v>5.5350000000000001</v>
+        <v>950</v>
       </c>
       <c r="E14">
-        <f>1.1*F14</f>
-        <v>6.7650000000000006</v>
+        <v>1050</v>
       </c>
       <c r="F14">
-        <v>6.15</v>
+        <v>1000</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1079,17 +1078,17 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D19" si="3">0.9*F15</f>
+        <f>0.9*F15</f>
         <v>5.5350000000000001</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E15:E19" si="4">1.1*F15</f>
+        <f>1.1*F15</f>
         <v>6.7650000000000006</v>
       </c>
       <c r="F15">
@@ -1105,17 +1104,17 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D16:D20" si="3">0.9*F16</f>
         <v>5.5350000000000001</v>
       </c>
       <c r="E16">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E16:E20" si="4">1.1*F16</f>
         <v>6.7650000000000006</v>
       </c>
       <c r="F16">
@@ -1131,10 +1130,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <f t="shared" si="3"/>
@@ -1157,10 +1156,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <f t="shared" si="3"/>
@@ -1183,10 +1182,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19">
         <f t="shared" si="3"/>
@@ -1205,38 +1204,40 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>1+A19</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="D20">
-        <v>23</v>
+        <f t="shared" si="3"/>
+        <v>5.5350000000000001</v>
       </c>
       <c r="E20">
-        <v>25</v>
+        <f t="shared" si="4"/>
+        <v>6.7650000000000006</v>
       </c>
       <c r="F20">
-        <v>24</v>
+        <v>6.15</v>
       </c>
       <c r="H20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" ref="A21:A33" si="5">1+A20</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D21">
         <v>23</v>
@@ -1253,23 +1254,23 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
+        <v>92</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H22" t="s">
         <v>9</v>
@@ -1277,23 +1278,23 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23">
-        <v>15.8</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>16.2</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H23" t="s">
         <v>9</v>
@@ -1301,23 +1302,23 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24">
-        <v>280</v>
+        <v>15.8</v>
       </c>
       <c r="E24">
-        <v>300</v>
+        <v>16.2</v>
       </c>
       <c r="F24">
-        <v>290</v>
+        <v>16</v>
       </c>
       <c r="H24" t="s">
         <v>9</v>
@@ -1325,23 +1326,23 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>57</v>
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
       </c>
       <c r="D25">
-        <v>238</v>
+        <v>280</v>
       </c>
       <c r="E25">
-        <v>242</v>
+        <v>300</v>
       </c>
       <c r="F25">
-        <v>240</v>
+        <v>290</v>
       </c>
       <c r="H25" t="s">
         <v>9</v>
@@ -1349,83 +1350,83 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>43</v>
+        <v>24</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D26">
-        <v>0.8</v>
+        <v>236</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>242</v>
       </c>
       <c r="F26">
-        <v>0.9</v>
+        <v>240</v>
       </c>
       <c r="H26" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>56</v>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27">
+        <v>0.8</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0.9</v>
       </c>
       <c r="H27" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0.2</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
+      <c r="C28" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="H28" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D29">
-        <v>4.8</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>5.0999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="F29">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H29" t="s">
         <v>9</v>
@@ -1433,23 +1434,23 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="E30">
-        <v>0.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30" t="s">
         <v>9</v>
@@ -1457,23 +1458,23 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31">
-        <v>4.8</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>5.0999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="F31">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H31" t="s">
         <v>9</v>
@@ -1481,23 +1482,23 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="E32">
-        <v>0.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H32" t="s">
         <v>9</v>
@@ -1505,25 +1506,49 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0.2</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="H33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
         <v>49</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>48</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>4.8</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F33">
+      <c r="F34">
         <v>5</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1537,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CEAD3C-E293-403D-9957-624DD4ECBBD6}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,7 +1606,7 @@
         <v>201</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>24.5</v>
@@ -1604,7 +1629,7 @@
         <v>202</v>
       </c>
       <c r="C3">
-        <v>23.5</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>24.5</v>
@@ -1627,7 +1652,7 @@
         <v>203</v>
       </c>
       <c r="C4">
-        <v>23.5</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>24.5</v>
@@ -1650,7 +1675,7 @@
         <v>204</v>
       </c>
       <c r="C5">
-        <v>23.5</v>
+        <v>19.5</v>
       </c>
       <c r="D5">
         <v>24.5</v>

</xml_diff>

<commit_message>
2 hardware issues: buck current is measuring as negative, and the FLT_OUT signal is not doing the right thing.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
+++ b/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761AEDA7-9F7A-445F-88CE-9536020F8CF4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8233D6-AC7E-4189-852F-69BC82E6C598}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
@@ -697,12 +697,12 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
@@ -1264,13 +1264,13 @@
         <v>94</v>
       </c>
       <c r="D22">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="E22">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="F22">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="H22" t="s">
         <v>9</v>
@@ -1420,13 +1420,13 @@
         <v>44</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="E29">
-        <v>0.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H29" t="s">
         <v>9</v>
@@ -1444,13 +1444,13 @@
         <v>45</v>
       </c>
       <c r="D30">
-        <v>4.8</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>5.0999999999999996</v>
+        <v>0.3</v>
       </c>
       <c r="F30">
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="H30" t="s">
         <v>9</v>
@@ -1516,13 +1516,13 @@
         <v>55</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="E33">
-        <v>0.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H33" t="s">
         <v>9</v>
@@ -1540,13 +1540,13 @@
         <v>48</v>
       </c>
       <c r="D34">
-        <v>4.8</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>5.0999999999999996</v>
+        <v>0.3</v>
       </c>
       <c r="F34">
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="H34" t="s">
         <v>9</v>
@@ -1563,7 +1563,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,10 +1813,10 @@
         <v>211</v>
       </c>
       <c r="C11">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="D11">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E11">
         <v>240</v>

</xml_diff>

<commit_message>
the notebook can run through completely, prompting for a DUT serial number, and writing results to a csv. DUT run time is ~ 8 minutes.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
+++ b/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8233D6-AC7E-4189-852F-69BC82E6C598}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461D5023-ABD8-4564-95D5-61DC02F81010}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
   <si>
     <t>TEST #</t>
   </si>
@@ -318,13 +318,10 @@
     <t>HvBuckBootstrap2</t>
   </si>
   <si>
-    <t>RL1</t>
-  </si>
-  <si>
-    <t>RL2</t>
-  </si>
-  <si>
     <t>HV CAP REGULATION</t>
+  </si>
+  <si>
+    <t>FlybackRegulation</t>
   </si>
 </sst>
 </file>
@@ -343,18 +340,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -375,10 +366,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -694,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA788C9-474B-4068-A04A-775EAB4B4CD4}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +699,7 @@
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -740,39 +730,33 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <f>0.95*F2</f>
         <v>19.170999999999999</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <f>1.05*F2</f>
         <v>21.189</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>20.18</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>1+A2</f>
         <v>1</v>
@@ -780,25 +764,25 @@
       <c r="B3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D9" si="0">0.95*F3</f>
         <v>19.170999999999999</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <f t="shared" ref="E3:E9" si="1">1.05*F3</f>
         <v>21.189</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>20.18</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A34" si="2">1+A3</f>
         <v>2</v>
@@ -806,25 +790,25 @@
       <c r="B4" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
         <v>28.689999999999998</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" si="1"/>
         <v>31.71</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>30.2</v>
       </c>
       <c r="H4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -832,25 +816,25 @@
       <c r="B5" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>28.689999999999998</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" si="1"/>
         <v>31.71</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>30.2</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -858,25 +842,25 @@
       <c r="B6" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
         <v>19.170999999999999</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" si="1"/>
         <v>21.189</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>20.18</v>
       </c>
       <c r="H6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -884,25 +868,25 @@
       <c r="B7" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>19.170999999999999</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="1"/>
         <v>21.189</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>20.18</v>
       </c>
       <c r="H7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -910,25 +894,25 @@
       <c r="B8" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>28.689999999999998</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="1"/>
         <v>31.71</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>30.2</v>
       </c>
       <c r="H8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -936,25 +920,25 @@
       <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>28.689999999999998</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f t="shared" si="1"/>
         <v>31.71</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>30.2</v>
       </c>
       <c r="H9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -978,7 +962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -986,7 +970,7 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D11">
@@ -1002,7 +986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1017,24 +1001,26 @@
         <v>310</v>
       </c>
       <c r="E12">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="F12">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="H12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="D13">
         <v>0.1</v>
       </c>
@@ -1048,7 +1034,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -1056,7 +1042,7 @@
       <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D14">
@@ -1072,7 +1058,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -1080,7 +1066,7 @@
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D15">
@@ -1098,7 +1084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -1106,7 +1092,7 @@
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D16">
@@ -1132,7 +1118,7 @@
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D17">
@@ -1158,7 +1144,7 @@
       <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D18">
@@ -1184,7 +1170,7 @@
       <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D19">
@@ -1210,7 +1196,7 @@
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D20">
@@ -1236,7 +1222,7 @@
       <c r="B21" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>93</v>
       </c>
       <c r="D21">
@@ -1260,7 +1246,7 @@
       <c r="B22" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D22">
@@ -1284,7 +1270,7 @@
       <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D23">
@@ -1308,7 +1294,7 @@
       <c r="B24" t="s">
         <v>20</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D24">
@@ -1332,7 +1318,7 @@
       <c r="B25" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D25">
@@ -1380,7 +1366,7 @@
       <c r="B27" t="s">
         <v>22</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D27">
@@ -1416,7 +1402,7 @@
       <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D29">
@@ -1440,7 +1426,7 @@
       <c r="B30" t="s">
         <v>29</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D30">
@@ -1464,7 +1450,7 @@
       <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D31">

</xml_diff>

<commit_message>
A very productive week! I should probably split this repo up. The front end gui for the power board is working well, next step is to think more about the back end and the actual testing.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
+++ b/PWRAutomatedTest/PWR_Board_TestReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461D5023-ABD8-4564-95D5-61DC02F81010}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B696CDEC-E39C-4D0C-B661-4F443B9B22B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="Quantities" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -687,7 +688,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,13 +999,13 @@
         <v>53</v>
       </c>
       <c r="D12">
+        <v>300</v>
+      </c>
+      <c r="E12">
+        <v>350</v>
+      </c>
+      <c r="F12">
         <v>310</v>
-      </c>
-      <c r="E12">
-        <v>325</v>
-      </c>
-      <c r="F12">
-        <v>317</v>
       </c>
       <c r="H12" t="s">
         <v>9</v>
@@ -1346,7 +1347,7 @@
         <v>57</v>
       </c>
       <c r="D26">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E26">
         <v>242</v>
@@ -1370,13 +1371,13 @@
         <v>43</v>
       </c>
       <c r="D27">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F27">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="H27" t="s">
         <v>23</v>
@@ -1549,7 +1550,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,13 +1777,13 @@
         <v>210</v>
       </c>
       <c r="C10">
+        <v>300</v>
+      </c>
+      <c r="D10">
+        <v>320</v>
+      </c>
+      <c r="E10">
         <v>310</v>
-      </c>
-      <c r="D10">
-        <v>325</v>
-      </c>
-      <c r="E10">
-        <v>315</v>
       </c>
       <c r="G10">
         <v>4</v>
@@ -1799,7 +1800,7 @@
         <v>211</v>
       </c>
       <c r="C11">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D11">
         <v>245</v>

</xml_diff>